<commit_message>
[CMSA-306] [웅진 Toolchain 인프라] Toolchain 공통 인프라 구성 - IaC
[Resolution]
기존 iac directory 구조 변경
elb를 vpc와 같은 level로 재구성
중복 변수 정리

[DoD]
terraform init, plan, apply를 통해서 각 resource가 생성되는지 확인

[Team]
Automation

[Company]
BespinGlobal
</commit_message>
<xml_diff>
--- a/site/docs/웅진 Toolchain 아키텍처 명세서.xlsx
+++ b/site/docs/웅진 Toolchain 아키텍처 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1442FD-D5AC-478E-9CE9-C40F3DA81FCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5852BE-9686-42B5-B025-E3CBE70CD45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37800" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37820" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t>Service</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,10 +227,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pub</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -279,10 +275,6 @@
   </si>
   <si>
     <t>-lc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AWS Cloud Sample Architecture service.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -350,19 +342,6 @@
   <si>
     <t>- Vpc : comp-apne2-def-vpc 
 - Subnet : pub-1a-sn</t>
-  </si>
-  <si>
-    <t>- Routing : comp-apne2-def-nat 
-- Subnet :  
-comp-apne2-prod-mgmt-1a-sn
-comp-apne2-prod-mgmt-1c-sn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>- Routing : comp-apne2-def-igw 
-- Subnet :  
-comp-apne2-prod-pub-1a-sn
-comp-apne2-prod-pub-1c-sn</t>
   </si>
   <si>
     <t xml:space="preserve">- Target_type : instance
@@ -373,31 +352,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>- Listener : SSH 22
-- Rules: comp-apne2-prod-gitlab-ssh-tg22
-- Listener : HTTP 80
-- Rules: comp-apne2-prod-gitlab-tg80 
-- Listener : HTTPS 443
-- Rules: comp-apne2-prod-gitlab-tg80</t>
-  </si>
-  <si>
-    <t>- Listener : HTTPS 443 
-- Rules: sonarqube.mingming.shop &gt; comp-apne2-prod-sonarqube-tg9000
-- Rules: jenkins.mingming.shop &gt; comp-apne2-prod-jenkins-tg8088
-- Rules: scm.mingming.shop &gt; comp-apne2-prod-scm-tg8088
-- Rules: nexus.mingming.shop &gt; comp-apne2-prod-nexus-tg8088</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>nexus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>scm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sonarqube</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -425,14 +384,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">- Target_type : instance
-- Vpc_id : _self
-- Protocol : HTTP
-- Port : 9000
-- Depends_on : mgmt-alb </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gitlab-ssh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -464,9 +415,60 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>- Inbound : HTTP 80 
+    <t>prod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Routing : comp-apne2-def-igw 
+- Subnet :  
+  comp-apne2-prod-pub-1a-sn
+  comp-apne2-prod-pub-1c-sn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Routing : comp-apne2-def-nat 
+- Subnet :  
+  comp-apne2-prod-mgmt-1a-sn
+  comp-apne2-prod-mgmt-1c-sn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Listener : SSH 22
+  Rules: comp-apne2-prod-gitlab-ssh-tg22
+- Listener : HTTP 80
+  Rules: comp-apne2-prod-gitlab-tg80
+- Listener : HTTPS 443
+  Rules: comp-apne2-prod-gitlab-tg80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWS Cloud Sample Architecture service.</t>
+  </si>
+  <si>
+    <t>scouter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">- Target_type : instance
+- Vpc_id : _self
+- Protocol : HTTP
+- Port : 6100
+- Depends_on : mgmt-alb </t>
+  </si>
+  <si>
+    <t>- Inbound : HTTP 6100 
 - Outbound : Anywhere</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Listener : HTTPS 443 
+  Rules: (host) scouter.mingming.shop &gt; (tg) comp-apne2-prod-scouter-tg
+  Rules: (host) jenkins.mingming.shop &gt; (tg) comp-apne2-prod-jenkins-tg
+  Rules: (host) scm.mingming.shop &gt; (tg) comp-apne2-prod-scm-tg
+  Rules: (host) nexus.mingming.shop &gt; (tg) comp-apne2-prod-nexus-tg</t>
+  </si>
+  <si>
+    <t>scouter</t>
   </si>
 </sst>
 </file>
@@ -933,16 +935,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="18.5" x14ac:dyDescent="1"/>
   <cols>
     <col min="2" max="2" width="13.53515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.69140625" customWidth="1"/>
-    <col min="4" max="4" width="27.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.4609375" customWidth="1"/>
+    <col min="4" max="4" width="29.84375" customWidth="1"/>
+    <col min="5" max="5" width="72.765625" customWidth="1"/>
     <col min="6" max="6" width="20.3828125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.84375" customWidth="1"/>
     <col min="8" max="8" width="16.3046875" customWidth="1"/>
@@ -951,12 +953,12 @@
     <col min="11" max="11" width="17.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="1">
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="1">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -964,15 +966,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="1">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -980,25 +982,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="1">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="1">
       <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="1">
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="10" spans="2:9" ht="52.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" ht="55.5" x14ac:dyDescent="1">
       <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1021,7 +1023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="1">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1030,118 +1032,118 @@
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" ref="D11:D32" si="0">CONCATENATE($H11,$C11,$I11)</f>
-        <v>comp-apne2-def-vpc</v>
+        <v>comp-apne2-prod-vpc</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1"/>
       <c r="H11" s="2" t="str">
         <f>VLOOKUP($B11,Rule!$B$3:$D$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I11" s="2" t="str">
         <f>VLOOKUP($B11,Rule!$B$3:$D$23,3,FALSE)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="70" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" ht="74" x14ac:dyDescent="1">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-pub-1a-sn</v>
+        <v>comp-apne2-prod-pub-1a-sn</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F12" s="1"/>
       <c r="H12" s="2" t="str">
         <f>VLOOKUP($B12,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I12" s="2" t="str">
         <f>VLOOKUP($B12,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sn</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="70" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" ht="74" x14ac:dyDescent="1">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-pub-1c-sn</v>
+        <v>comp-apne2-prod-pub-1c-sn</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F13" s="1"/>
       <c r="H13" s="2" t="str">
         <f>VLOOKUP($B13,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I13" s="2" t="str">
         <f>VLOOKUP($B13,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sn</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="70" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" ht="74" x14ac:dyDescent="1">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-mgmt-1a-sn</v>
+        <v>comp-apne2-prod-mgmt-1a-sn</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1"/>
       <c r="H14" s="2" t="str">
         <f>VLOOKUP($B14,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I14" s="2" t="str">
         <f>VLOOKUP($B14,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sn</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="70" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" ht="74" x14ac:dyDescent="1">
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-mgmt-1c-sn</v>
+        <v>comp-apne2-prod-mgmt-1c-sn</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F15" s="1"/>
       <c r="H15" s="2" t="str">
         <f>VLOOKUP($B15,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I15" s="2" t="str">
         <f>VLOOKUP($B15,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sn</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="1">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1150,19 +1152,19 @@
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-igw</v>
+        <v>comp-apne2-prod-igw</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F16" s="1"/>
       <c r="H16" s="2" t="str">
         <f>VLOOKUP($B16,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" ht="35" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" ht="37" x14ac:dyDescent="1">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1171,436 +1173,436 @@
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-nat</v>
+        <v>comp-apne2-prod-nat</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1"/>
       <c r="H17" s="2" t="str">
         <f>VLOOKUP($B17,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" ht="70" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" ht="74" x14ac:dyDescent="1">
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-pub-rt</v>
+        <v>comp-apne2-prod-pub-rt</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F18" s="1"/>
       <c r="H18" s="2" t="str">
         <f>VLOOKUP($B18,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I18" s="2" t="str">
         <f>VLOOKUP($B18,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-rt</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="70" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" ht="74" x14ac:dyDescent="1">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-pri-rt</v>
+        <v>comp-apne2-prod-pri-rt</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F19" s="1"/>
       <c r="H19" s="2" t="str">
         <f>VLOOKUP($B19,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I19" s="2" t="str">
         <f>VLOOKUP($B19,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-rt</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="140" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" ht="111" x14ac:dyDescent="1">
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-apne2-def-gitlab-nlb</v>
+        <v>comp-apne2-prod-gitlab-nlb</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F20" s="1"/>
       <c r="H20" s="2" t="str">
         <f>VLOOKUP($B20,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21" s="1" t="str">
-        <f>CONCATENATE($H21,$C21,$I21)</f>
-        <v>comp-apne2-def-mgmt-alb</v>
+        <f t="shared" ref="D21:D31" si="1">CONCATENATE($H21,$C21,$I21)</f>
+        <v>comp-apne2-prod-mgmt-alb</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F21" s="1"/>
       <c r="H21" s="2" t="str">
         <f>VLOOKUP($B21,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1" t="str">
-        <f>CONCATENATE($H22,$C22,$I22)</f>
-        <v>comp-apne2-def-gitlab-tg</v>
+        <f t="shared" si="1"/>
+        <v>comp-apne2-prod-gitlab-tg</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F22" s="1"/>
       <c r="H22" s="2" t="str">
         <f>VLOOKUP($B22,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I22" s="2" t="str">
         <f>VLOOKUP($B22,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-tg</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D23" s="1" t="str">
-        <f>CONCATENATE($H23,$C23,$I23)</f>
-        <v>comp-apne2-def-gitlab-ssh-tg</v>
+        <f t="shared" si="1"/>
+        <v>comp-apne2-prod-gitlab-ssh-tg</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F23" s="1"/>
       <c r="H23" s="2" t="str">
         <f>VLOOKUP($B23,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I23" s="2" t="str">
         <f>VLOOKUP($B23,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-tg</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1" t="str">
-        <f>CONCATENATE($H24,$C24,$I24)</f>
-        <v>comp-apne2-def-jenkins-tg</v>
+        <f t="shared" si="1"/>
+        <v>comp-apne2-prod-jenkins-tg</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F24" s="1"/>
       <c r="H24" s="2" t="str">
         <f>VLOOKUP($B24,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I24" s="2" t="str">
         <f>VLOOKUP($B24,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-tg</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f>CONCATENATE($H25,$C25,$I25)</f>
-        <v>comp-apne2-def-nexus-tg</v>
+        <f t="shared" si="1"/>
+        <v>comp-apne2-prod-nexus-tg</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F25" s="1"/>
       <c r="H25" s="2" t="str">
         <f>VLOOKUP($B25,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I25" s="2" t="str">
         <f>VLOOKUP($B25,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-tg</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f>CONCATENATE($H26,$C26,$I26)</f>
-        <v>comp-apne2-def-scm-tg</v>
+        <f t="shared" si="1"/>
+        <v>comp-apne2-prod-scm-tg</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F26" s="1"/>
       <c r="H26" s="2" t="str">
         <f>VLOOKUP($B26,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I26" s="2" t="str">
         <f>VLOOKUP($B26,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-tg</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="87.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" ht="92.5" x14ac:dyDescent="1">
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f>CONCATENATE($H27,$C27,$I27)</f>
-        <v>comp-apne2-def-sonarqube-tg</v>
+        <f t="shared" si="1"/>
+        <v>comp-apne2-prod-scouter-tg</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F27" s="1"/>
       <c r="H27" s="2" t="str">
         <f>VLOOKUP($B27,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="I27" s="2" t="str">
         <f>VLOOKUP($B27,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-tg</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="1">
       <c r="B28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f>CONCATENATE($H28,$C28,$I28)</f>
-        <v>comp-def-default-ops-sg-sg</v>
+        <f t="shared" si="1"/>
+        <v>comp-prod-default-ops-sg-sg</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F28" s="1"/>
       <c r="H28" s="2" t="str">
         <f>VLOOKUP($B28,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I28" s="2" t="str">
         <f>VLOOKUP($B28,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sg</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="35" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" ht="37" x14ac:dyDescent="1">
       <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1" t="str">
-        <f>CONCATENATE($H29,$C29,$I29)</f>
-        <v>comp-def-gitlab-sg</v>
+        <f t="shared" si="1"/>
+        <v>comp-prod-gitlab-sg</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F29" s="1"/>
       <c r="H29" s="2" t="str">
         <f>VLOOKUP($B29,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I29" s="2" t="str">
         <f>VLOOKUP($B29,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sg</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="35" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" ht="37" x14ac:dyDescent="1">
       <c r="B30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f>CONCATENATE($H30,$C30,$I30)</f>
-        <v>comp-def-mgmt-alb-sg</v>
+        <f t="shared" si="1"/>
+        <v>comp-prod-mgmt-alb-sg</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F30" s="1"/>
       <c r="H30" s="2" t="str">
         <f>VLOOKUP($B30,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I30" s="2" t="str">
         <f>VLOOKUP($B30,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sg</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="35" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" ht="37" x14ac:dyDescent="1">
       <c r="B31" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f>CONCATENATE($H31,$C31,$I31)</f>
-        <v>comp-def-jenkins-sg</v>
+        <f t="shared" si="1"/>
+        <v>comp-prod-jenkins-sg</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F31" s="1"/>
       <c r="H31" s="2" t="str">
         <f>VLOOKUP($B31,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I31" s="2" t="str">
         <f>VLOOKUP($B31,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sg</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="35" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" ht="37" x14ac:dyDescent="1">
       <c r="B32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>comp-def-sonarqube-sg</v>
+        <v>comp-prod-scouter-sg</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="1"/>
       <c r="H32" s="2" t="str">
         <f>VLOOKUP($B32,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I32" s="2" t="str">
         <f>VLOOKUP($B32,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-sg</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:9" x14ac:dyDescent="1">
       <c r="B33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="str">
         <f>CONCATENATE($H33,$C33,$I33)</f>
-        <v>comp-def-jenkins-ec2</v>
+        <v>comp-prod-jenkins-ec2</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" s="2" t="str">
         <f>VLOOKUP($B33,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I33" s="2" t="str">
         <f>VLOOKUP($B33,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-ec2</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:9" x14ac:dyDescent="1">
       <c r="B34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>CONCATENATE($H34,$C34,$I34)</f>
-        <v>comp-def-gitlab-ec2</v>
+        <v>comp-prod-gitlab-ec2</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="H34" s="2" t="str">
         <f>VLOOKUP($B34,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I34" s="2" t="str">
         <f>VLOOKUP($B34,Rule!$B$3:$D$23,3,FALSE)</f>
         <v>-ec2</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:9" x14ac:dyDescent="1">
       <c r="B35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D35" s="1" t="str">
         <f>CONCATENATE($H35,$C35,$I35)</f>
-        <v>comp-def-sonarqube-ec2</v>
+        <v>comp-prod-scouter-ec2</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="H35" s="2" t="str">
         <f>VLOOKUP($B35,Rule!$B$3:$C$23,2,FALSE)</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="I35" s="2" t="str">
         <f>VLOOKUP($B35,Rule!$B$3:$D$23,3,FALSE)</f>
@@ -1612,7 +1614,7 @@
     <mergeCell ref="B7:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B35" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>유형</formula1>
     </dataValidation>
@@ -1630,14 +1632,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="18.5" x14ac:dyDescent="1"/>
   <cols>
     <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="1">
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
@@ -1648,220 +1650,220 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="1">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="1">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="1">
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="1">
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="1">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="1">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$6,"-")</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="1">
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="1">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="1">
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="1">
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="1">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="1">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",,project!$C$6,"-")</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="1">
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",,project!$C$6,"-")</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="1">
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" x14ac:dyDescent="1">
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" x14ac:dyDescent="1">
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",project!$C$5,"-",project!$C$6,"-")</f>
-        <v>comp-apne2-def-</v>
+        <v>comp-apne2-prod-</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="1">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>CONCATENATE(project!$C$4,"-",,project!$C$6,"-")</f>
-        <v>comp-def-</v>
+        <v>comp-prod-</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="1">
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="1">
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1870,7 +1872,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="1">
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1879,7 +1881,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" x14ac:dyDescent="1">
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>